<commit_message>
BOT; UPDATE DATA (#150)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/sodan.xlsx
+++ b/static/data/sodan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\216212\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file.kobe.local\top\02_作業文書\01_組織\平成31年度\01_市長室\03_広報戦略部\01_広報課\04_HP\コロナ\HP作図\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="＿" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$79</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$82</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -503,13 +503,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A62" sqref="A62:XFD62"/>
+      <selection pane="bottomRight" activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1760,17 +1760,68 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="3"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
+      <c r="A74" s="3">
+        <v>43929</v>
+      </c>
+      <c r="B74" s="5">
+        <v>938</v>
+      </c>
+      <c r="C74" s="5">
+        <v>17734</v>
+      </c>
+      <c r="D74" s="4">
+        <v>158</v>
+      </c>
+      <c r="E74" s="4">
+        <v>4546</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="3"/>
-      <c r="B75" s="5" t="s">
+      <c r="A75" s="3">
+        <v>43930</v>
+      </c>
+      <c r="B75" s="5">
+        <v>892</v>
+      </c>
+      <c r="C75" s="5">
+        <v>18626</v>
+      </c>
+      <c r="D75" s="4">
+        <v>171</v>
+      </c>
+      <c r="E75" s="4">
+        <v>4735</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" s="3">
+        <v>43931</v>
+      </c>
+      <c r="B76" s="5">
+        <v>926</v>
+      </c>
+      <c r="C76" s="5">
+        <v>19552</v>
+      </c>
+      <c r="D76" s="4">
+        <v>137</v>
+      </c>
+      <c r="E76" s="4">
+        <v>4872</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" s="3"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A78" s="3"/>
+      <c r="B78" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#211)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/sodan.xlsx
+++ b/static/data/sodan.xlsx
@@ -16,7 +16,7 @@
     <sheet name="＿" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$83</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$84</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -503,13 +503,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E78" sqref="E78"/>
+      <selection pane="bottomRight" activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1845,12 +1845,29 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="3"/>
-      <c r="B79" s="5" t="s">
+      <c r="A79" s="3">
+        <v>43934</v>
+      </c>
+      <c r="B79" s="5">
+        <v>1047</v>
+      </c>
+      <c r="C79" s="5">
+        <v>22005</v>
+      </c>
+      <c r="D79" s="4">
+        <v>195</v>
+      </c>
+      <c r="E79" s="4">
+        <v>5067</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A80" s="3"/>
+      <c r="B80" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#340)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/sodan.xlsx
+++ b/static/data/sodan.xlsx
@@ -16,7 +16,7 @@
     <sheet name="＿" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$88</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$89</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -520,13 +520,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E83" sqref="E83"/>
+      <selection pane="bottomRight" activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1947,12 +1947,29 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A84" s="3"/>
-      <c r="B84" s="5" t="s">
+      <c r="A84" s="3">
+        <v>43939</v>
+      </c>
+      <c r="B84" s="7">
+        <v>522</v>
+      </c>
+      <c r="C84" s="7">
+        <v>25457</v>
+      </c>
+      <c r="D84" s="9">
+        <v>0</v>
+      </c>
+      <c r="E84" s="8">
+        <v>5665</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A85" s="3"/>
+      <c r="B85" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#367)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/sodan.xlsx
+++ b/static/data/sodan.xlsx
@@ -520,13 +520,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C85" sqref="C85"/>
+      <selection pane="bottomRight" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1964,12 +1964,26 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A85" s="3"/>
-      <c r="B85" s="5" t="s">
+      <c r="A85" s="3">
+        <v>43940</v>
+      </c>
+      <c r="B85" s="5">
+        <v>523</v>
+      </c>
+      <c r="C85" s="5">
+        <v>25980</v>
+      </c>
+      <c r="D85" s="4">
+        <v>0</v>
+      </c>
+      <c r="E85" s="4">
+        <v>5665</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B86" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#458)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/sodan.xlsx
+++ b/static/data/sodan.xlsx
@@ -16,9 +16,9 @@
     <sheet name="＿" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$92</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$93</definedName>
   </definedNames>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -498,13 +498,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
+      <selection pane="bottomRight" activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2013,17 +2013,28 @@
       <c r="A89" s="3">
         <v>43944</v>
       </c>
-      <c r="B89" s="7"/>
+      <c r="B89" s="7">
+        <v>561</v>
+      </c>
       <c r="C89" s="7">
-        <v>27820</v>
-      </c>
-      <c r="D89" s="8"/>
+        <v>28381</v>
+      </c>
+      <c r="D89" s="8">
+        <v>159</v>
+      </c>
       <c r="E89" s="8">
-        <v>6195</v>
+        <v>6354</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B90" s="5" t="s">
+      <c r="A90" s="3"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B91" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#530)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/sodan.xlsx
+++ b/static/data/sodan.xlsx
@@ -16,7 +16,7 @@
     <sheet name="＿" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$94</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$95</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -498,13 +498,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E93" sqref="E93"/>
+      <selection pane="bottomRight" activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2047,13 +2047,30 @@
       <c r="A91" s="3">
         <v>43946</v>
       </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
+      <c r="B91" s="7">
+        <v>524</v>
+      </c>
+      <c r="C91" s="7">
+        <v>29514</v>
+      </c>
+      <c r="D91" s="8">
+        <v>0</v>
+      </c>
+      <c r="E91" s="8">
+        <v>6458</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B92" s="5" t="s">
+      <c r="A92" s="3">
+        <v>43947</v>
+      </c>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B93" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#531)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/sodan.xlsx
+++ b/static/data/sodan.xlsx
@@ -16,7 +16,7 @@
     <sheet name="＿" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$94</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$95</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -498,13 +498,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E93" sqref="E93"/>
+      <selection pane="bottomRight" activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2047,13 +2047,30 @@
       <c r="A91" s="3">
         <v>43946</v>
       </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
+      <c r="B91" s="7">
+        <v>524</v>
+      </c>
+      <c r="C91" s="7">
+        <v>29514</v>
+      </c>
+      <c r="D91" s="8">
+        <v>0</v>
+      </c>
+      <c r="E91" s="8">
+        <v>6458</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B92" s="5" t="s">
+      <c r="A92" s="3">
+        <v>43947</v>
+      </c>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B93" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#776)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/sodan.xlsx
+++ b/static/data/sodan.xlsx
@@ -16,7 +16,7 @@
     <sheet name="＿" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$98</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$99</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -498,13 +498,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A95" sqref="A95"/>
+      <selection pane="bottomRight" activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2129,7 +2129,24 @@
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B96" s="5" t="s">
+      <c r="A96" s="3">
+        <v>43951</v>
+      </c>
+      <c r="B96" s="7">
+        <v>792</v>
+      </c>
+      <c r="C96" s="7">
+        <v>32302</v>
+      </c>
+      <c r="D96" s="8">
+        <v>185</v>
+      </c>
+      <c r="E96" s="8">
+        <v>6849</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B97" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#777)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/sodan.xlsx
+++ b/static/data/sodan.xlsx
@@ -16,7 +16,7 @@
     <sheet name="＿" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$98</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$99</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -498,13 +498,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A95" sqref="A95"/>
+      <selection pane="bottomRight" activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2129,7 +2129,24 @@
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B96" s="5" t="s">
+      <c r="A96" s="3">
+        <v>43951</v>
+      </c>
+      <c r="B96" s="7">
+        <v>792</v>
+      </c>
+      <c r="C96" s="7">
+        <v>32302</v>
+      </c>
+      <c r="D96" s="8">
+        <v>185</v>
+      </c>
+      <c r="E96" s="8">
+        <v>6849</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B97" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BOT; UPDATE DATA (#1914)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/static/data/sodan.xlsx
+++ b/static/data/sodan.xlsx
@@ -16,7 +16,7 @@
     <sheet name="＿" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$123</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">相談件数!$A$1:$E$124</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -498,13 +498,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C131" sqref="C131"/>
+      <selection pane="bottomRight" activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2588,8 +2588,25 @@
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A123" s="3"/>
-      <c r="B123" s="5" t="s">
+      <c r="A123" s="3">
+        <v>43978</v>
+      </c>
+      <c r="B123" s="7">
+        <v>132</v>
+      </c>
+      <c r="C123" s="7">
+        <v>39307</v>
+      </c>
+      <c r="D123" s="8">
+        <v>38</v>
+      </c>
+      <c r="E123" s="8">
+        <v>7912</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A124" s="3"/>
+      <c r="B124" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>